<commit_message>
Updated Class Diagram and Initial Sprint 3 Backlog
Updated the class diagram to correctly present the current state of the application. Updated the sprint backlog to include overview trip item functionality.
</commit_message>
<xml_diff>
--- a/sprints/sprint3/Sprint Backlog - Sprint 3 Initial.xlsx
+++ b/sprints/sprint3/Sprint Backlog - Sprint 3 Initial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aznel\Documents\UWG\2021-2022\spring semester\capstone\CS4982Project\sprints\sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE01A5A4-0145-4F75-B1B1-7E0B835B605C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822EC382-2800-4E99-BA2F-06A2020D315E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Features</t>
   </si>
@@ -76,10 +76,16 @@
     <t>Testing - DAL</t>
   </si>
   <si>
-    <t>UI Web - Validation</t>
+    <t>Web - Events Bugs</t>
   </si>
   <si>
-    <t>UI Web - Events Bugs</t>
+    <t>Web - Validation</t>
+  </si>
+  <si>
+    <t>UI Desktop - View Trip Item</t>
+  </si>
+  <si>
+    <t>UI Web - View Trip Item</t>
   </si>
 </sst>
 </file>
@@ -158,11 +164,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -352,51 +355,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$12:$P$12</c:f>
+              <c:f>Sheet1!$C$10:$P$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1249,7 +1213,7 @@
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1541,240 +1505,240 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="6"/>
-    <col min="3" max="16" width="9.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="41.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="5"/>
+    <col min="3" max="16" width="9.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="1">
         <v>44260</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>44261</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>44262</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>44263</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>44264</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
         <v>44265</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>44266</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="1">
         <v>44267</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="1">
         <v>44268</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="1">
         <v>44269</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="1">
         <v>44270</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="1">
         <v>44271</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="1">
         <v>44272</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="1">
         <v>44273</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>3</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>5</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>5</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" s="3">
         <v>5</v>
@@ -1794,109 +1758,157 @@
       <c r="P9" s="3"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>5</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="4">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2">
         <v>5</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1">
-        <f>SUM(C3:C11)</f>
-        <v>31</v>
-      </c>
-      <c r="D12" s="7">
-        <f t="shared" ref="D12:P12" si="0">SUM(D3:D11)</f>
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3">
+        <v>5</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="4">
+        <v>5</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6">
+        <f>SUM(C3:C13)</f>
+        <v>41</v>
+      </c>
+      <c r="D14" s="6">
+        <f t="shared" ref="D14:P14" si="0">SUM(D3:D13)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E14" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F14" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G14" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H14" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I14" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J14" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K14" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L14" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M14" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N14" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O14" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P14" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1906,6 +1918,7 @@
     <mergeCell ref="C1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>